<commit_message>
Fixed grammar and spelling mistakes in report
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chart2" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>4,4,43533,5250</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Tile Space</t>
+  </si>
+  <si>
+    <t>DFS Randomised</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -207,7 +209,7 @@
             <c:numRef>
               <c:f>Sheet2!$K$5:$K$9</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>43533</c:v>
@@ -308,7 +310,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>312</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>947</c:v>
@@ -385,11 +387,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1803524112"/>
-        <c:axId val="1803521936"/>
+        <c:axId val="882070496"/>
+        <c:axId val="882063424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1803524112"/>
+        <c:axId val="882070496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,7 +433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1803521936"/>
+        <c:crossAx val="882063424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -439,7 +441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1803521936"/>
+        <c:axId val="882063424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -459,7 +461,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -490,7 +492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1803524112"/>
+        <c:crossAx val="882070496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -504,7 +506,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -581,7 +582,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -646,7 +646,7 @@
             <c:numRef>
               <c:f>Sheet2!$K$5:$K$9</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>43533</c:v>
@@ -747,7 +747,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>312</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>947</c:v>
@@ -824,11 +824,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1616850736"/>
-        <c:axId val="1616860528"/>
+        <c:axId val="882069952"/>
+        <c:axId val="882059616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1616850736"/>
+        <c:axId val="882069952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +870,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1616860528"/>
+        <c:crossAx val="882059616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -878,7 +878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1616860528"/>
+        <c:axId val="882059616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +898,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -929,7 +929,740 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1616850736"/>
+        <c:crossAx val="882069952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Nodes Expanded for Various Search Methods, against tile space of board</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Depth-First Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$5:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$K$5:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43533</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90815</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>284735</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>168092</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Breadth-First Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$5:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$L$5:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3829</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6718</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9073</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9708</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$M$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iterative Deepening</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$5:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$M$5:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>947</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1235</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1412</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1532</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heuristic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$5:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$N$5:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4354</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4609</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$O$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DFS Randomised</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$O$5:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>27741</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>162902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>605686</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="704417904"/>
+        <c:axId val="704418448"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="704417904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>No. Of Tiles In Board </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="704418448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="704418448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Nodes Expanded</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="704417904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1002,6 +1735,1224 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Average Nodes Expanded for Various Search Methods, against tile space of board</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Breadth-First Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$5:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$L$5:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3829</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6718</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9073</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9708</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$M$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iterative Deepening</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$5:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$M$5:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>947</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1235</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1412</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1532</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heuristic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$5:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$N$5:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4354</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4609</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1004229168"/>
+        <c:axId val="1004216656"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1004229168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>No of Tiles In</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Board</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1004216656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1004216656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Nodes Expanded</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1004229168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Agent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Moves for various search methods, against tile space of board</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11237270341207348"/>
+          <c:y val="0.18560185185185185"/>
+          <c:w val="0.84596062992125987"/>
+          <c:h val="0.54380322251385238"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$K$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Depth-First Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$13:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$K$13:$K$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20883</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118908</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>397432</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>248592</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>167392</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$L$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Breadth-First Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$13:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$L$13:$L$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$M$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iterative Deepening</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$13:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$M$13:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$N$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heuristic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$J$13:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$N$13:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1378631520"/>
+        <c:axId val="1378633152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1378631520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1378633152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1378633152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1378631520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1085,6 +3036,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1738,6 +3809,1554 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2164,6 +5783,101 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2430,10 +6144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N25"/>
+  <dimension ref="A3:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,9 +6157,10 @@
     <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -2460,13 +6175,13 @@
         <v>43533</v>
       </c>
       <c r="E3">
-        <v>5250</v>
+        <v>20883</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -2481,7 +6196,7 @@
         <v>90815</v>
       </c>
       <c r="E4">
-        <v>88728</v>
+        <v>118908</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>10</v>
@@ -2498,8 +6213,11 @@
       <c r="N4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="O4" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>6</v>
       </c>
@@ -2514,13 +6232,13 @@
         <v>284735</v>
       </c>
       <c r="E5">
-        <v>279010</v>
+        <v>397432</v>
       </c>
       <c r="J5" s="2">
         <f>$C$3</f>
         <v>16</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5">
         <f>D3</f>
         <v>43533</v>
       </c>
@@ -2529,15 +6247,17 @@
         <v>3829</v>
       </c>
       <c r="M5" s="3">
-        <f>D15</f>
-        <v>312</v>
+        <v>266</v>
       </c>
       <c r="N5" s="3">
         <f>D21</f>
         <v>3629</v>
       </c>
+      <c r="O5">
+        <v>27741</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -2558,7 +6278,7 @@
         <f>$C$4</f>
         <v>25</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6">
         <f t="shared" ref="K6:K9" si="0">D4</f>
         <v>90815</v>
       </c>
@@ -2574,8 +6294,11 @@
         <f t="shared" ref="N6:N9" si="3">D22</f>
         <v>3007</v>
       </c>
+      <c r="O6">
+        <v>162902</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -2596,7 +6319,7 @@
         <f>$C$5</f>
         <v>36</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7">
         <f t="shared" si="0"/>
         <v>284735</v>
       </c>
@@ -2612,13 +6335,16 @@
         <f t="shared" si="3"/>
         <v>3585</v>
       </c>
+      <c r="O7">
+        <v>605686</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J8" s="2">
         <f>$C$6</f>
         <v>49</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8">
         <f t="shared" si="0"/>
         <v>250667</v>
       </c>
@@ -2635,7 +6361,7 @@
         <v>4354</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2656,7 +6382,7 @@
         <f>$C$7</f>
         <v>64</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>168092</v>
       </c>
@@ -2673,7 +6399,7 @@
         <v>4609</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -2691,7 +6417,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -2712,7 +6438,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -2742,7 +6468,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -2765,7 +6491,7 @@
       </c>
       <c r="K13" s="3">
         <f>E3</f>
-        <v>5250</v>
+        <v>20883</v>
       </c>
       <c r="L13" s="3">
         <f>E9</f>
@@ -2780,14 +6506,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J14" s="2">
         <f>$C$4</f>
         <v>25</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" ref="K14:K17" si="4">E4</f>
-        <v>88728</v>
+        <v>118908</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" ref="L14:L17" si="5">E10</f>
@@ -2802,7 +6528,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -2814,7 +6540,7 @@
         <v>16</v>
       </c>
       <c r="D15">
-        <v>312</v>
+        <v>266</v>
       </c>
       <c r="E15">
         <v>16</v>
@@ -2825,7 +6551,7 @@
       </c>
       <c r="K15" s="3">
         <f t="shared" si="4"/>
-        <v>279010</v>
+        <v>397432</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" si="5"/>
@@ -2840,7 +6566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -3045,6 +6771,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>